<commit_message>
contestants who are judges
</commit_message>
<xml_diff>
--- a/Data/Beat_Bobby_Flay_Wikipedia_Data.xlsx
+++ b/Data/Beat_Bobby_Flay_Wikipedia_Data.xlsx
@@ -4172,9 +4172,6 @@
     <t>Robert Sisca, Michael Brennan</t>
   </si>
   <si>
-    <t>Frank Pellegrino, Jr., Rosanna Scotto, Ed McFarland</t>
-  </si>
-  <si>
     <t>Bouillabaisse</t>
   </si>
   <si>
@@ -6474,6 +6471,9 @@
   </si>
   <si>
     <t>Curtis Stone, Haylie Duff</t>
+  </si>
+  <si>
+    <t>Frank Pellegrino Jr., Rosanna Scotto, Ed McFarland</t>
   </si>
 </sst>
 </file>
@@ -6802,9 +6802,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F107" sqref="F107"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I196" sqref="I196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6823,37 +6823,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2120</v>
+      </c>
+      <c r="B1" t="s">
         <v>2121</v>
       </c>
-      <c r="B1" t="s">
-        <v>2122</v>
-      </c>
       <c r="C1" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="F1" t="s">
+        <v>2122</v>
+      </c>
+      <c r="G1" t="s">
         <v>2123</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2124</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2125</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2126</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2127</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2128</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6993,7 +6993,7 @@
         <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -8113,7 +8113,7 @@
         <v>258</v>
       </c>
       <c r="K37" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -8463,7 +8463,7 @@
         <v>328</v>
       </c>
       <c r="K47" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -8953,7 +8953,7 @@
         <v>427</v>
       </c>
       <c r="K61" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -9058,7 +9058,7 @@
         <v>448</v>
       </c>
       <c r="K64" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -9478,7 +9478,7 @@
         <v>534</v>
       </c>
       <c r="K76" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -9618,7 +9618,7 @@
         <v>562</v>
       </c>
       <c r="K80" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -9653,7 +9653,7 @@
         <v>569</v>
       </c>
       <c r="K81" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -9863,7 +9863,7 @@
         <v>611</v>
       </c>
       <c r="K87" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -9968,7 +9968,7 @@
         <v>630</v>
       </c>
       <c r="K90" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -10108,7 +10108,7 @@
         <v>659</v>
       </c>
       <c r="K94" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -10248,7 +10248,7 @@
         <v>686</v>
       </c>
       <c r="K98" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -10548,7 +10548,7 @@
         <v>747</v>
       </c>
       <c r="F107" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="G107" t="s">
         <v>748</v>
@@ -10732,7 +10732,7 @@
         <v>785</v>
       </c>
       <c r="I112" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="J112" t="s">
         <v>786</v>
@@ -10808,7 +10808,7 @@
         <v>799</v>
       </c>
       <c r="K114" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
@@ -12803,7 +12803,7 @@
         <v>1204</v>
       </c>
       <c r="K171" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
@@ -13529,7 +13529,7 @@
         <v>1352</v>
       </c>
       <c r="H192" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="I192" t="s">
         <v>1353</v>
@@ -13599,7 +13599,7 @@
         <v>1366</v>
       </c>
       <c r="H194" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="I194" t="s">
         <v>1367</v>
@@ -13672,13 +13672,13 @@
         <v>1381</v>
       </c>
       <c r="I196" t="s">
+        <v>2149</v>
+      </c>
+      <c r="J196" t="s">
         <v>1382</v>
       </c>
-      <c r="J196" t="s">
+      <c r="K196" t="s">
         <v>1383</v>
-      </c>
-      <c r="K196" t="s">
-        <v>1384</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
@@ -13692,25 +13692,25 @@
         <v>11</v>
       </c>
       <c r="D197" t="s">
+        <v>1384</v>
+      </c>
+      <c r="E197" s="1" t="s">
         <v>1385</v>
       </c>
-      <c r="E197" s="1" t="s">
+      <c r="F197" t="s">
         <v>1386</v>
       </c>
-      <c r="F197" t="s">
+      <c r="G197" t="s">
         <v>1387</v>
       </c>
-      <c r="G197" t="s">
+      <c r="H197" t="s">
         <v>1388</v>
       </c>
-      <c r="H197" t="s">
+      <c r="I197" t="s">
         <v>1389</v>
       </c>
-      <c r="I197" t="s">
+      <c r="J197" t="s">
         <v>1390</v>
-      </c>
-      <c r="J197" t="s">
-        <v>1391</v>
       </c>
       <c r="K197" t="s">
         <v>16</v>
@@ -13727,28 +13727,28 @@
         <v>12</v>
       </c>
       <c r="D198" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E198" s="1" t="s">
         <v>1392</v>
       </c>
-      <c r="E198" s="1" t="s">
+      <c r="F198" t="s">
         <v>1393</v>
       </c>
-      <c r="F198" t="s">
+      <c r="G198" t="s">
         <v>1394</v>
       </c>
-      <c r="G198" t="s">
+      <c r="H198" t="s">
         <v>1395</v>
       </c>
-      <c r="H198" t="s">
+      <c r="I198" t="s">
         <v>1396</v>
       </c>
-      <c r="I198" t="s">
+      <c r="J198" t="s">
         <v>1397</v>
       </c>
-      <c r="J198" t="s">
+      <c r="K198" t="s">
         <v>1398</v>
-      </c>
-      <c r="K198" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
@@ -13762,25 +13762,25 @@
         <v>13</v>
       </c>
       <c r="D199" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E199" s="1" t="s">
         <v>1400</v>
       </c>
-      <c r="E199" s="1" t="s">
+      <c r="F199" t="s">
         <v>1401</v>
       </c>
-      <c r="F199" t="s">
+      <c r="G199" t="s">
         <v>1402</v>
       </c>
-      <c r="G199" t="s">
+      <c r="H199" t="s">
         <v>1403</v>
       </c>
-      <c r="H199" t="s">
+      <c r="I199" t="s">
         <v>1404</v>
       </c>
-      <c r="I199" t="s">
+      <c r="J199" t="s">
         <v>1405</v>
-      </c>
-      <c r="J199" t="s">
-        <v>1406</v>
       </c>
       <c r="K199" t="s">
         <v>16</v>
@@ -13797,25 +13797,25 @@
         <v>1</v>
       </c>
       <c r="D200" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E200" s="1" t="s">
         <v>1407</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="F200" t="s">
         <v>1408</v>
       </c>
-      <c r="F200" t="s">
+      <c r="G200" t="s">
         <v>1409</v>
       </c>
-      <c r="G200" t="s">
+      <c r="H200" t="s">
         <v>1410</v>
       </c>
-      <c r="H200" t="s">
+      <c r="I200" t="s">
         <v>1411</v>
       </c>
-      <c r="I200" t="s">
+      <c r="J200" t="s">
         <v>1412</v>
-      </c>
-      <c r="J200" t="s">
-        <v>1413</v>
       </c>
       <c r="K200" t="s">
         <v>16</v>
@@ -13832,28 +13832,28 @@
         <v>2</v>
       </c>
       <c r="D201" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E201" s="1" t="s">
         <v>1414</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="F201" t="s">
         <v>1415</v>
       </c>
-      <c r="F201" t="s">
+      <c r="G201" t="s">
         <v>1416</v>
       </c>
-      <c r="G201" t="s">
+      <c r="H201" t="s">
         <v>1417</v>
       </c>
-      <c r="H201" t="s">
+      <c r="I201" t="s">
         <v>1418</v>
       </c>
-      <c r="I201" t="s">
+      <c r="J201" t="s">
         <v>1419</v>
       </c>
-      <c r="J201" t="s">
+      <c r="K201" t="s">
         <v>1420</v>
-      </c>
-      <c r="K201" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
@@ -13867,25 +13867,25 @@
         <v>3</v>
       </c>
       <c r="D202" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E202" s="1" t="s">
         <v>1422</v>
       </c>
-      <c r="E202" s="1" t="s">
+      <c r="F202" t="s">
         <v>1423</v>
       </c>
-      <c r="F202" t="s">
+      <c r="G202" t="s">
         <v>1424</v>
       </c>
-      <c r="G202" t="s">
+      <c r="H202" t="s">
         <v>1425</v>
       </c>
-      <c r="H202" t="s">
+      <c r="I202" t="s">
         <v>1426</v>
       </c>
-      <c r="I202" t="s">
+      <c r="J202" t="s">
         <v>1427</v>
-      </c>
-      <c r="J202" t="s">
-        <v>1428</v>
       </c>
       <c r="K202" t="s">
         <v>16</v>
@@ -13902,28 +13902,28 @@
         <v>4</v>
       </c>
       <c r="D203" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E203" s="1" t="s">
         <v>1429</v>
       </c>
-      <c r="E203" s="1" t="s">
+      <c r="F203" t="s">
         <v>1430</v>
       </c>
-      <c r="F203" t="s">
+      <c r="G203" t="s">
         <v>1431</v>
       </c>
-      <c r="G203" t="s">
+      <c r="H203" t="s">
         <v>1432</v>
       </c>
-      <c r="H203" t="s">
+      <c r="I203" t="s">
         <v>1433</v>
       </c>
-      <c r="I203" t="s">
+      <c r="J203" t="s">
         <v>1434</v>
       </c>
-      <c r="J203" t="s">
+      <c r="K203" t="s">
         <v>1435</v>
-      </c>
-      <c r="K203" t="s">
-        <v>1436</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
@@ -13937,25 +13937,25 @@
         <v>5</v>
       </c>
       <c r="D204" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E204" s="1" t="s">
         <v>1437</v>
       </c>
-      <c r="E204" s="1" t="s">
+      <c r="F204" t="s">
         <v>1438</v>
       </c>
-      <c r="F204" t="s">
+      <c r="G204" t="s">
         <v>1439</v>
       </c>
-      <c r="G204" t="s">
+      <c r="H204" t="s">
         <v>1440</v>
       </c>
-      <c r="H204" t="s">
+      <c r="I204" t="s">
         <v>1441</v>
       </c>
-      <c r="I204" t="s">
+      <c r="J204" t="s">
         <v>1442</v>
-      </c>
-      <c r="J204" t="s">
-        <v>1443</v>
       </c>
       <c r="K204" t="s">
         <v>16</v>
@@ -13972,28 +13972,28 @@
         <v>6</v>
       </c>
       <c r="D205" t="s">
+        <v>1443</v>
+      </c>
+      <c r="E205" s="1" t="s">
         <v>1444</v>
       </c>
-      <c r="E205" s="1" t="s">
+      <c r="F205" t="s">
         <v>1445</v>
       </c>
-      <c r="F205" t="s">
+      <c r="G205" t="s">
         <v>1446</v>
       </c>
-      <c r="G205" t="s">
+      <c r="H205" t="s">
         <v>1447</v>
       </c>
-      <c r="H205" t="s">
+      <c r="I205" t="s">
         <v>1448</v>
       </c>
-      <c r="I205" t="s">
+      <c r="J205" t="s">
         <v>1449</v>
       </c>
-      <c r="J205" t="s">
+      <c r="K205" t="s">
         <v>1450</v>
-      </c>
-      <c r="K205" t="s">
-        <v>1451</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
@@ -14007,25 +14007,25 @@
         <v>7</v>
       </c>
       <c r="D206" t="s">
+        <v>1451</v>
+      </c>
+      <c r="E206" s="1" t="s">
         <v>1452</v>
       </c>
-      <c r="E206" s="1" t="s">
+      <c r="F206" t="s">
         <v>1453</v>
       </c>
-      <c r="F206" t="s">
+      <c r="G206" t="s">
         <v>1454</v>
       </c>
-      <c r="G206" t="s">
+      <c r="H206" t="s">
         <v>1455</v>
       </c>
-      <c r="H206" t="s">
+      <c r="I206" t="s">
         <v>1456</v>
       </c>
-      <c r="I206" t="s">
+      <c r="J206" t="s">
         <v>1457</v>
-      </c>
-      <c r="J206" t="s">
-        <v>1458</v>
       </c>
       <c r="K206" t="s">
         <v>16</v>
@@ -14042,25 +14042,25 @@
         <v>8</v>
       </c>
       <c r="D207" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E207" s="1" t="s">
         <v>1459</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="F207" t="s">
         <v>1460</v>
       </c>
-      <c r="F207" t="s">
+      <c r="G207" t="s">
         <v>1461</v>
       </c>
-      <c r="G207" t="s">
+      <c r="H207" t="s">
         <v>1462</v>
       </c>
-      <c r="H207" t="s">
+      <c r="I207" t="s">
         <v>1463</v>
       </c>
-      <c r="I207" t="s">
+      <c r="J207" t="s">
         <v>1464</v>
-      </c>
-      <c r="J207" t="s">
-        <v>1465</v>
       </c>
       <c r="K207" t="s">
         <v>16</v>
@@ -14077,25 +14077,25 @@
         <v>9</v>
       </c>
       <c r="D208" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E208" s="1" t="s">
         <v>1466</v>
       </c>
-      <c r="E208" s="1" t="s">
+      <c r="F208" t="s">
         <v>1467</v>
       </c>
-      <c r="F208" t="s">
+      <c r="G208" t="s">
         <v>1468</v>
       </c>
-      <c r="G208" t="s">
+      <c r="H208" t="s">
         <v>1469</v>
       </c>
-      <c r="H208" t="s">
+      <c r="I208" t="s">
         <v>1470</v>
       </c>
-      <c r="I208" t="s">
+      <c r="J208" t="s">
         <v>1471</v>
-      </c>
-      <c r="J208" t="s">
-        <v>1472</v>
       </c>
       <c r="K208" t="s">
         <v>16</v>
@@ -14112,28 +14112,28 @@
         <v>10</v>
       </c>
       <c r="D209" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E209" s="1" t="s">
         <v>1473</v>
       </c>
-      <c r="E209" s="1" t="s">
+      <c r="F209" t="s">
         <v>1474</v>
       </c>
-      <c r="F209" t="s">
+      <c r="G209" t="s">
         <v>1475</v>
       </c>
-      <c r="G209" t="s">
+      <c r="H209" t="s">
         <v>1476</v>
       </c>
-      <c r="H209" t="s">
+      <c r="I209" t="s">
         <v>1477</v>
       </c>
-      <c r="I209" t="s">
+      <c r="J209" t="s">
         <v>1478</v>
       </c>
-      <c r="J209" t="s">
+      <c r="K209" t="s">
         <v>1479</v>
-      </c>
-      <c r="K209" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
@@ -14147,25 +14147,25 @@
         <v>11</v>
       </c>
       <c r="D210" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E210" s="1" t="s">
         <v>1481</v>
       </c>
-      <c r="E210" s="1" t="s">
+      <c r="F210" t="s">
         <v>1482</v>
       </c>
-      <c r="F210" t="s">
+      <c r="G210" t="s">
         <v>1483</v>
       </c>
-      <c r="G210" t="s">
+      <c r="H210" t="s">
         <v>1484</v>
       </c>
-      <c r="H210" t="s">
+      <c r="I210" t="s">
         <v>1485</v>
       </c>
-      <c r="I210" t="s">
+      <c r="J210" t="s">
         <v>1486</v>
-      </c>
-      <c r="J210" t="s">
-        <v>1487</v>
       </c>
       <c r="K210" t="s">
         <v>16</v>
@@ -14182,28 +14182,28 @@
         <v>12</v>
       </c>
       <c r="D211" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E211" s="1" t="s">
         <v>1488</v>
       </c>
-      <c r="E211" s="1" t="s">
+      <c r="F211" t="s">
         <v>1489</v>
       </c>
-      <c r="F211" t="s">
+      <c r="G211" t="s">
         <v>1490</v>
       </c>
-      <c r="G211" t="s">
+      <c r="H211" t="s">
         <v>1491</v>
       </c>
-      <c r="H211" t="s">
+      <c r="I211" t="s">
         <v>1492</v>
       </c>
-      <c r="I211" t="s">
+      <c r="J211" t="s">
         <v>1493</v>
       </c>
-      <c r="J211" t="s">
+      <c r="K211" t="s">
         <v>1494</v>
-      </c>
-      <c r="K211" t="s">
-        <v>1495</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
@@ -14217,25 +14217,25 @@
         <v>13</v>
       </c>
       <c r="D212" t="s">
+        <v>1495</v>
+      </c>
+      <c r="E212" s="1" t="s">
         <v>1496</v>
       </c>
-      <c r="E212" s="1" t="s">
+      <c r="F212" t="s">
         <v>1497</v>
       </c>
-      <c r="F212" t="s">
+      <c r="G212" t="s">
         <v>1498</v>
       </c>
-      <c r="G212" t="s">
+      <c r="H212" t="s">
         <v>1499</v>
       </c>
-      <c r="H212" t="s">
+      <c r="I212" t="s">
         <v>1500</v>
       </c>
-      <c r="I212" t="s">
+      <c r="J212" t="s">
         <v>1501</v>
-      </c>
-      <c r="J212" t="s">
-        <v>1502</v>
       </c>
       <c r="K212" t="s">
         <v>16</v>
@@ -14252,25 +14252,25 @@
         <v>1</v>
       </c>
       <c r="D213" t="s">
+        <v>1502</v>
+      </c>
+      <c r="E213" s="1" t="s">
         <v>1503</v>
       </c>
-      <c r="E213" s="1" t="s">
+      <c r="F213" t="s">
         <v>1504</v>
       </c>
-      <c r="F213" t="s">
+      <c r="G213" t="s">
         <v>1505</v>
       </c>
-      <c r="G213" t="s">
+      <c r="H213" t="s">
         <v>1506</v>
       </c>
-      <c r="H213" t="s">
+      <c r="I213" t="s">
         <v>1507</v>
       </c>
-      <c r="I213" t="s">
+      <c r="J213" t="s">
         <v>1508</v>
-      </c>
-      <c r="J213" t="s">
-        <v>1509</v>
       </c>
       <c r="K213" t="s">
         <v>16</v>
@@ -14287,28 +14287,28 @@
         <v>2</v>
       </c>
       <c r="D214" t="s">
+        <v>1509</v>
+      </c>
+      <c r="E214" s="1" t="s">
         <v>1510</v>
       </c>
-      <c r="E214" s="1" t="s">
+      <c r="F214" t="s">
         <v>1511</v>
       </c>
-      <c r="F214" t="s">
+      <c r="G214" t="s">
         <v>1512</v>
       </c>
-      <c r="G214" t="s">
+      <c r="H214" t="s">
         <v>1513</v>
       </c>
-      <c r="H214" t="s">
+      <c r="I214" t="s">
         <v>1514</v>
       </c>
-      <c r="I214" t="s">
+      <c r="J214" t="s">
         <v>1515</v>
       </c>
-      <c r="J214" t="s">
+      <c r="K214" t="s">
         <v>1516</v>
-      </c>
-      <c r="K214" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
@@ -14322,25 +14322,25 @@
         <v>3</v>
       </c>
       <c r="D215" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E215" s="1" t="s">
         <v>1518</v>
       </c>
-      <c r="E215" s="1" t="s">
+      <c r="F215" t="s">
         <v>1519</v>
       </c>
-      <c r="F215" t="s">
+      <c r="G215" t="s">
         <v>1520</v>
       </c>
-      <c r="G215" t="s">
+      <c r="H215" t="s">
         <v>1521</v>
       </c>
-      <c r="H215" t="s">
+      <c r="I215" t="s">
         <v>1522</v>
       </c>
-      <c r="I215" t="s">
+      <c r="J215" t="s">
         <v>1523</v>
-      </c>
-      <c r="J215" t="s">
-        <v>1524</v>
       </c>
       <c r="K215" t="s">
         <v>16</v>
@@ -14357,25 +14357,25 @@
         <v>4</v>
       </c>
       <c r="D216" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E216" s="1" t="s">
         <v>1525</v>
       </c>
-      <c r="E216" s="1" t="s">
+      <c r="F216" t="s">
         <v>1526</v>
       </c>
-      <c r="F216" t="s">
+      <c r="G216" t="s">
         <v>1527</v>
       </c>
-      <c r="G216" t="s">
+      <c r="H216" t="s">
         <v>1528</v>
       </c>
-      <c r="H216" t="s">
+      <c r="I216" t="s">
         <v>1529</v>
       </c>
-      <c r="I216" t="s">
+      <c r="J216" t="s">
         <v>1530</v>
-      </c>
-      <c r="J216" t="s">
-        <v>1531</v>
       </c>
       <c r="K216" t="s">
         <v>16</v>
@@ -14392,28 +14392,28 @@
         <v>5</v>
       </c>
       <c r="D217" t="s">
+        <v>1531</v>
+      </c>
+      <c r="E217" s="1" t="s">
         <v>1532</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="F217" t="s">
         <v>1533</v>
       </c>
-      <c r="F217" t="s">
+      <c r="G217" t="s">
         <v>1534</v>
       </c>
-      <c r="G217" t="s">
+      <c r="H217" t="s">
         <v>1535</v>
       </c>
-      <c r="H217" t="s">
+      <c r="I217" t="s">
         <v>1536</v>
       </c>
-      <c r="I217" t="s">
+      <c r="J217" t="s">
         <v>1537</v>
       </c>
-      <c r="J217" t="s">
+      <c r="K217" t="s">
         <v>1538</v>
-      </c>
-      <c r="K217" t="s">
-        <v>1539</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
@@ -14427,25 +14427,25 @@
         <v>6</v>
       </c>
       <c r="D218" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E218" s="1" t="s">
         <v>1540</v>
       </c>
-      <c r="E218" s="1" t="s">
+      <c r="F218" t="s">
         <v>1541</v>
       </c>
-      <c r="F218" t="s">
+      <c r="G218" t="s">
         <v>1542</v>
       </c>
-      <c r="G218" t="s">
+      <c r="H218" t="s">
         <v>1543</v>
       </c>
-      <c r="H218" t="s">
+      <c r="I218" t="s">
         <v>1544</v>
       </c>
-      <c r="I218" t="s">
+      <c r="J218" t="s">
         <v>1545</v>
-      </c>
-      <c r="J218" t="s">
-        <v>1546</v>
       </c>
       <c r="K218" t="s">
         <v>16</v>
@@ -14462,25 +14462,25 @@
         <v>7</v>
       </c>
       <c r="D219" t="s">
+        <v>1546</v>
+      </c>
+      <c r="E219" s="1" t="s">
         <v>1547</v>
       </c>
-      <c r="E219" s="1" t="s">
+      <c r="F219" t="s">
         <v>1548</v>
       </c>
-      <c r="F219" t="s">
+      <c r="G219" t="s">
         <v>1549</v>
       </c>
-      <c r="G219" t="s">
+      <c r="H219" t="s">
         <v>1550</v>
       </c>
-      <c r="H219" t="s">
+      <c r="I219" t="s">
         <v>1551</v>
       </c>
-      <c r="I219" t="s">
+      <c r="J219" t="s">
         <v>1552</v>
-      </c>
-      <c r="J219" t="s">
-        <v>1553</v>
       </c>
       <c r="K219" t="s">
         <v>16</v>
@@ -14497,25 +14497,25 @@
         <v>8</v>
       </c>
       <c r="D220" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E220" s="1" t="s">
         <v>1554</v>
       </c>
-      <c r="E220" s="1" t="s">
+      <c r="F220" t="s">
         <v>1555</v>
       </c>
-      <c r="F220" t="s">
+      <c r="G220" t="s">
         <v>1556</v>
       </c>
-      <c r="G220" t="s">
+      <c r="H220" t="s">
         <v>1557</v>
       </c>
-      <c r="H220" t="s">
+      <c r="I220" t="s">
         <v>1558</v>
       </c>
-      <c r="I220" t="s">
+      <c r="J220" t="s">
         <v>1559</v>
-      </c>
-      <c r="J220" t="s">
-        <v>1560</v>
       </c>
       <c r="K220" t="s">
         <v>16</v>
@@ -14532,28 +14532,28 @@
         <v>9</v>
       </c>
       <c r="D221" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E221" s="1" t="s">
         <v>1561</v>
       </c>
-      <c r="E221" s="1" t="s">
+      <c r="F221" t="s">
         <v>1562</v>
       </c>
-      <c r="F221" t="s">
+      <c r="G221" t="s">
         <v>1563</v>
       </c>
-      <c r="G221" t="s">
+      <c r="H221" t="s">
         <v>1564</v>
       </c>
-      <c r="H221" t="s">
+      <c r="I221" t="s">
         <v>1565</v>
       </c>
-      <c r="I221" t="s">
+      <c r="J221" t="s">
         <v>1566</v>
       </c>
-      <c r="J221" t="s">
+      <c r="K221" t="s">
         <v>1567</v>
-      </c>
-      <c r="K221" t="s">
-        <v>1568</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
@@ -14567,25 +14567,25 @@
         <v>10</v>
       </c>
       <c r="D222" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E222" s="1" t="s">
         <v>1569</v>
       </c>
-      <c r="E222" s="1" t="s">
+      <c r="F222" t="s">
         <v>1570</v>
       </c>
-      <c r="F222" t="s">
+      <c r="G222" t="s">
         <v>1571</v>
       </c>
-      <c r="G222" t="s">
+      <c r="H222" t="s">
         <v>1572</v>
       </c>
-      <c r="H222" t="s">
+      <c r="I222" t="s">
         <v>1573</v>
       </c>
-      <c r="I222" t="s">
+      <c r="J222" t="s">
         <v>1574</v>
-      </c>
-      <c r="J222" t="s">
-        <v>1575</v>
       </c>
       <c r="K222" t="s">
         <v>16</v>
@@ -14602,25 +14602,25 @@
         <v>11</v>
       </c>
       <c r="D223" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>1576</v>
       </c>
-      <c r="E223" s="1" t="s">
+      <c r="F223" t="s">
         <v>1577</v>
       </c>
-      <c r="F223" t="s">
+      <c r="G223" t="s">
         <v>1578</v>
       </c>
-      <c r="G223" t="s">
+      <c r="H223" t="s">
         <v>1579</v>
       </c>
-      <c r="H223" t="s">
+      <c r="I223" t="s">
         <v>1580</v>
       </c>
-      <c r="I223" t="s">
+      <c r="J223" t="s">
         <v>1581</v>
-      </c>
-      <c r="J223" t="s">
-        <v>1582</v>
       </c>
       <c r="K223" t="s">
         <v>16</v>
@@ -14637,25 +14637,25 @@
         <v>12</v>
       </c>
       <c r="D224" t="s">
+        <v>1582</v>
+      </c>
+      <c r="E224" s="1" t="s">
         <v>1583</v>
       </c>
-      <c r="E224" s="1" t="s">
+      <c r="F224" t="s">
         <v>1584</v>
       </c>
-      <c r="F224" t="s">
+      <c r="G224" t="s">
         <v>1585</v>
       </c>
-      <c r="G224" t="s">
+      <c r="H224" t="s">
         <v>1586</v>
       </c>
-      <c r="H224" t="s">
+      <c r="I224" t="s">
         <v>1587</v>
       </c>
-      <c r="I224" t="s">
+      <c r="J224" t="s">
         <v>1588</v>
-      </c>
-      <c r="J224" t="s">
-        <v>1589</v>
       </c>
       <c r="K224" t="s">
         <v>16</v>
@@ -14672,25 +14672,25 @@
         <v>13</v>
       </c>
       <c r="D225" t="s">
+        <v>1589</v>
+      </c>
+      <c r="E225" s="1" t="s">
         <v>1590</v>
       </c>
-      <c r="E225" s="1" t="s">
+      <c r="F225" t="s">
         <v>1591</v>
       </c>
-      <c r="F225" t="s">
+      <c r="G225" t="s">
         <v>1592</v>
       </c>
-      <c r="G225" t="s">
+      <c r="H225" t="s">
         <v>1593</v>
       </c>
-      <c r="H225" t="s">
+      <c r="I225" t="s">
         <v>1594</v>
       </c>
-      <c r="I225" t="s">
+      <c r="J225" t="s">
         <v>1595</v>
-      </c>
-      <c r="J225" t="s">
-        <v>1596</v>
       </c>
       <c r="K225" t="s">
         <v>16</v>
@@ -14707,28 +14707,28 @@
         <v>14</v>
       </c>
       <c r="D226" t="s">
+        <v>1596</v>
+      </c>
+      <c r="E226" s="1" t="s">
         <v>1597</v>
       </c>
-      <c r="E226" s="1" t="s">
+      <c r="F226" t="s">
         <v>1598</v>
       </c>
-      <c r="F226" t="s">
+      <c r="G226" t="s">
         <v>1599</v>
       </c>
-      <c r="G226" t="s">
+      <c r="H226" t="s">
         <v>1600</v>
       </c>
-      <c r="H226" t="s">
+      <c r="I226" t="s">
         <v>1601</v>
       </c>
-      <c r="I226" t="s">
+      <c r="J226" t="s">
         <v>1602</v>
       </c>
-      <c r="J226" t="s">
+      <c r="K226" t="s">
         <v>1603</v>
-      </c>
-      <c r="K226" t="s">
-        <v>1604</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
@@ -14742,28 +14742,28 @@
         <v>1</v>
       </c>
       <c r="D227" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E227" s="1" t="s">
         <v>1605</v>
       </c>
-      <c r="E227" s="1" t="s">
+      <c r="F227" t="s">
         <v>1606</v>
       </c>
-      <c r="F227" t="s">
+      <c r="G227" t="s">
         <v>1607</v>
       </c>
-      <c r="G227" t="s">
+      <c r="H227" t="s">
         <v>1608</v>
       </c>
-      <c r="H227" t="s">
+      <c r="I227" t="s">
         <v>1609</v>
       </c>
-      <c r="I227" t="s">
+      <c r="J227" t="s">
         <v>1610</v>
       </c>
-      <c r="J227" t="s">
+      <c r="K227" t="s">
         <v>1611</v>
-      </c>
-      <c r="K227" t="s">
-        <v>1612</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
@@ -14777,28 +14777,28 @@
         <v>2</v>
       </c>
       <c r="D228" t="s">
+        <v>1612</v>
+      </c>
+      <c r="E228" s="1" t="s">
         <v>1613</v>
       </c>
-      <c r="E228" s="1" t="s">
+      <c r="F228" t="s">
         <v>1614</v>
       </c>
-      <c r="F228" t="s">
+      <c r="G228" t="s">
         <v>1615</v>
       </c>
-      <c r="G228" t="s">
+      <c r="H228" t="s">
         <v>1616</v>
       </c>
-      <c r="H228" t="s">
+      <c r="I228" t="s">
         <v>1617</v>
       </c>
-      <c r="I228" t="s">
+      <c r="J228" t="s">
         <v>1618</v>
       </c>
-      <c r="J228" t="s">
+      <c r="K228" t="s">
         <v>1619</v>
-      </c>
-      <c r="K228" t="s">
-        <v>1620</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
@@ -14812,28 +14812,28 @@
         <v>3</v>
       </c>
       <c r="D229" t="s">
+        <v>1620</v>
+      </c>
+      <c r="E229" s="1" t="s">
         <v>1621</v>
-      </c>
-      <c r="E229" s="1" t="s">
-        <v>1622</v>
       </c>
       <c r="F229" t="s">
         <v>1067</v>
       </c>
       <c r="G229" t="s">
+        <v>1622</v>
+      </c>
+      <c r="H229" t="s">
         <v>1623</v>
       </c>
-      <c r="H229" t="s">
+      <c r="I229" t="s">
         <v>1624</v>
       </c>
-      <c r="I229" t="s">
+      <c r="J229" t="s">
         <v>1625</v>
       </c>
-      <c r="J229" t="s">
+      <c r="K229" t="s">
         <v>1626</v>
-      </c>
-      <c r="K229" t="s">
-        <v>1627</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
@@ -14847,25 +14847,25 @@
         <v>4</v>
       </c>
       <c r="D230" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E230" s="1" t="s">
         <v>1628</v>
       </c>
-      <c r="E230" s="1" t="s">
+      <c r="F230" t="s">
         <v>1629</v>
       </c>
-      <c r="F230" t="s">
+      <c r="G230" t="s">
         <v>1630</v>
       </c>
-      <c r="G230" t="s">
+      <c r="H230" t="s">
         <v>1631</v>
       </c>
-      <c r="H230" t="s">
+      <c r="I230" t="s">
         <v>1632</v>
       </c>
-      <c r="I230" t="s">
+      <c r="J230" t="s">
         <v>1633</v>
-      </c>
-      <c r="J230" t="s">
-        <v>1634</v>
       </c>
       <c r="K230" t="s">
         <v>16</v>
@@ -14882,25 +14882,25 @@
         <v>5</v>
       </c>
       <c r="D231" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E231" s="1" t="s">
         <v>1635</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="F231" t="s">
         <v>1636</v>
       </c>
-      <c r="F231" t="s">
+      <c r="G231" t="s">
         <v>1637</v>
       </c>
-      <c r="G231" t="s">
+      <c r="H231" t="s">
         <v>1638</v>
       </c>
-      <c r="H231" t="s">
+      <c r="I231" t="s">
         <v>1639</v>
       </c>
-      <c r="I231" t="s">
+      <c r="J231" t="s">
         <v>1640</v>
-      </c>
-      <c r="J231" t="s">
-        <v>1641</v>
       </c>
       <c r="K231" t="s">
         <v>16</v>
@@ -14917,25 +14917,25 @@
         <v>6</v>
       </c>
       <c r="D232" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>1642</v>
       </c>
-      <c r="E232" s="1" t="s">
+      <c r="F232" t="s">
         <v>1643</v>
       </c>
-      <c r="F232" t="s">
+      <c r="G232" t="s">
         <v>1644</v>
       </c>
-      <c r="G232" t="s">
+      <c r="H232" t="s">
         <v>1645</v>
       </c>
-      <c r="H232" t="s">
+      <c r="I232" t="s">
         <v>1646</v>
       </c>
-      <c r="I232" t="s">
+      <c r="J232" t="s">
         <v>1647</v>
-      </c>
-      <c r="J232" t="s">
-        <v>1648</v>
       </c>
       <c r="K232" t="s">
         <v>16</v>
@@ -14952,25 +14952,25 @@
         <v>7</v>
       </c>
       <c r="D233" t="s">
+        <v>1648</v>
+      </c>
+      <c r="E233" s="1" t="s">
         <v>1649</v>
       </c>
-      <c r="E233" s="1" t="s">
+      <c r="F233" t="s">
         <v>1650</v>
       </c>
-      <c r="F233" t="s">
+      <c r="G233" t="s">
         <v>1651</v>
       </c>
-      <c r="G233" t="s">
+      <c r="H233" t="s">
         <v>1652</v>
       </c>
-      <c r="H233" t="s">
+      <c r="I233" t="s">
         <v>1653</v>
       </c>
-      <c r="I233" t="s">
+      <c r="J233" t="s">
         <v>1654</v>
-      </c>
-      <c r="J233" t="s">
-        <v>1655</v>
       </c>
       <c r="K233" t="s">
         <v>16</v>
@@ -14987,25 +14987,25 @@
         <v>8</v>
       </c>
       <c r="D234" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E234" s="1" t="s">
         <v>1656</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>1657</v>
       </c>
       <c r="F234" t="s">
         <v>105</v>
       </c>
       <c r="G234" t="s">
+        <v>1657</v>
+      </c>
+      <c r="H234" t="s">
         <v>1658</v>
       </c>
-      <c r="H234" t="s">
+      <c r="I234" t="s">
         <v>1659</v>
       </c>
-      <c r="I234" t="s">
+      <c r="J234" t="s">
         <v>1660</v>
-      </c>
-      <c r="J234" t="s">
-        <v>1661</v>
       </c>
       <c r="K234" t="s">
         <v>16</v>
@@ -15022,28 +15022,28 @@
         <v>9</v>
       </c>
       <c r="D235" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E235" s="1" t="s">
         <v>1662</v>
       </c>
-      <c r="E235" s="1" t="s">
+      <c r="F235" t="s">
         <v>1663</v>
       </c>
-      <c r="F235" t="s">
+      <c r="G235" t="s">
         <v>1664</v>
       </c>
-      <c r="G235" t="s">
+      <c r="H235" t="s">
         <v>1665</v>
       </c>
-      <c r="H235" t="s">
+      <c r="I235" t="s">
         <v>1666</v>
       </c>
-      <c r="I235" t="s">
+      <c r="J235" t="s">
         <v>1667</v>
       </c>
-      <c r="J235" t="s">
+      <c r="K235" t="s">
         <v>1668</v>
-      </c>
-      <c r="K235" t="s">
-        <v>1669</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
@@ -15057,25 +15057,25 @@
         <v>10</v>
       </c>
       <c r="D236" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E236" s="1" t="s">
         <v>1670</v>
       </c>
-      <c r="E236" s="1" t="s">
+      <c r="F236" t="s">
         <v>1671</v>
       </c>
-      <c r="F236" t="s">
+      <c r="G236" t="s">
         <v>1672</v>
       </c>
-      <c r="G236" t="s">
+      <c r="H236" t="s">
         <v>1673</v>
       </c>
-      <c r="H236" t="s">
+      <c r="I236" t="s">
         <v>1674</v>
       </c>
-      <c r="I236" t="s">
+      <c r="J236" t="s">
         <v>1675</v>
-      </c>
-      <c r="J236" t="s">
-        <v>1676</v>
       </c>
       <c r="K236" t="s">
         <v>16</v>
@@ -15092,28 +15092,28 @@
         <v>11</v>
       </c>
       <c r="D237" t="s">
+        <v>1676</v>
+      </c>
+      <c r="E237" s="1" t="s">
         <v>1677</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>1678</v>
       </c>
       <c r="F237" t="s">
         <v>444</v>
       </c>
       <c r="G237" t="s">
+        <v>1678</v>
+      </c>
+      <c r="H237" t="s">
         <v>1679</v>
       </c>
-      <c r="H237" t="s">
+      <c r="I237" t="s">
         <v>1680</v>
       </c>
-      <c r="I237" t="s">
+      <c r="J237" t="s">
         <v>1681</v>
       </c>
-      <c r="J237" t="s">
+      <c r="K237" t="s">
         <v>1682</v>
-      </c>
-      <c r="K237" t="s">
-        <v>1683</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
@@ -15127,25 +15127,25 @@
         <v>12</v>
       </c>
       <c r="D238" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>1684</v>
       </c>
-      <c r="E238" s="1" t="s">
+      <c r="F238" t="s">
         <v>1685</v>
       </c>
-      <c r="F238" t="s">
+      <c r="G238" t="s">
         <v>1686</v>
       </c>
-      <c r="G238" t="s">
+      <c r="H238" t="s">
         <v>1687</v>
       </c>
-      <c r="H238" t="s">
+      <c r="I238" t="s">
         <v>1688</v>
       </c>
-      <c r="I238" t="s">
+      <c r="J238" t="s">
         <v>1689</v>
-      </c>
-      <c r="J238" t="s">
-        <v>1690</v>
       </c>
       <c r="K238" t="s">
         <v>16</v>
@@ -15162,28 +15162,28 @@
         <v>1</v>
       </c>
       <c r="D239" t="s">
+        <v>1690</v>
+      </c>
+      <c r="E239" s="1" t="s">
         <v>1691</v>
       </c>
-      <c r="E239" s="1" t="s">
+      <c r="F239" t="s">
         <v>1692</v>
       </c>
-      <c r="F239" t="s">
+      <c r="G239" t="s">
         <v>1693</v>
       </c>
-      <c r="G239" t="s">
+      <c r="H239" t="s">
         <v>1694</v>
       </c>
-      <c r="H239" t="s">
+      <c r="I239" t="s">
         <v>1695</v>
       </c>
-      <c r="I239" t="s">
+      <c r="J239" t="s">
         <v>1696</v>
       </c>
-      <c r="J239" t="s">
+      <c r="K239" t="s">
         <v>1697</v>
-      </c>
-      <c r="K239" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
@@ -15197,25 +15197,25 @@
         <v>2</v>
       </c>
       <c r="D240" t="s">
+        <v>1698</v>
+      </c>
+      <c r="E240" s="1" t="s">
         <v>1699</v>
       </c>
-      <c r="E240" s="1" t="s">
+      <c r="F240" t="s">
         <v>1700</v>
       </c>
-      <c r="F240" t="s">
+      <c r="G240" t="s">
         <v>1701</v>
       </c>
-      <c r="G240" t="s">
+      <c r="H240" t="s">
         <v>1702</v>
       </c>
-      <c r="H240" t="s">
+      <c r="I240" t="s">
         <v>1703</v>
       </c>
-      <c r="I240" t="s">
+      <c r="J240" t="s">
         <v>1704</v>
-      </c>
-      <c r="J240" t="s">
-        <v>1705</v>
       </c>
       <c r="K240" t="s">
         <v>16</v>
@@ -15232,28 +15232,28 @@
         <v>3</v>
       </c>
       <c r="D241" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E241" s="1" t="s">
         <v>1706</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>1707</v>
       </c>
       <c r="F241" t="s">
         <v>61</v>
       </c>
       <c r="G241" t="s">
+        <v>1707</v>
+      </c>
+      <c r="H241" t="s">
         <v>1708</v>
       </c>
-      <c r="H241" t="s">
+      <c r="I241" t="s">
         <v>1709</v>
       </c>
-      <c r="I241" t="s">
+      <c r="J241" t="s">
         <v>1710</v>
       </c>
-      <c r="J241" t="s">
+      <c r="K241" t="s">
         <v>1711</v>
-      </c>
-      <c r="K241" t="s">
-        <v>1712</v>
       </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
@@ -15267,25 +15267,25 @@
         <v>4</v>
       </c>
       <c r="D242" t="s">
+        <v>1712</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>1713</v>
       </c>
-      <c r="E242" s="1" t="s">
+      <c r="F242" t="s">
         <v>1714</v>
       </c>
-      <c r="F242" t="s">
+      <c r="G242" t="s">
         <v>1715</v>
       </c>
-      <c r="G242" t="s">
+      <c r="H242" t="s">
         <v>1716</v>
       </c>
-      <c r="H242" t="s">
+      <c r="I242" t="s">
         <v>1717</v>
       </c>
-      <c r="I242" t="s">
+      <c r="J242" t="s">
         <v>1718</v>
-      </c>
-      <c r="J242" t="s">
-        <v>1719</v>
       </c>
       <c r="K242" t="s">
         <v>16</v>
@@ -15302,25 +15302,25 @@
         <v>5</v>
       </c>
       <c r="D243" t="s">
+        <v>1719</v>
+      </c>
+      <c r="E243" s="1" t="s">
         <v>1720</v>
       </c>
-      <c r="E243" s="1" t="s">
+      <c r="F243" t="s">
         <v>1721</v>
       </c>
-      <c r="F243" t="s">
+      <c r="G243" t="s">
         <v>1722</v>
       </c>
-      <c r="G243" t="s">
+      <c r="H243" t="s">
         <v>1723</v>
       </c>
-      <c r="H243" t="s">
+      <c r="I243" t="s">
         <v>1724</v>
       </c>
-      <c r="I243" t="s">
+      <c r="J243" t="s">
         <v>1725</v>
-      </c>
-      <c r="J243" t="s">
-        <v>1726</v>
       </c>
       <c r="K243" t="s">
         <v>16</v>
@@ -15337,28 +15337,28 @@
         <v>6</v>
       </c>
       <c r="D244" t="s">
+        <v>1726</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>1727</v>
       </c>
-      <c r="E244" s="1" t="s">
+      <c r="F244" t="s">
         <v>1728</v>
       </c>
-      <c r="F244" t="s">
+      <c r="G244" t="s">
         <v>1729</v>
       </c>
-      <c r="G244" t="s">
+      <c r="H244" t="s">
         <v>1730</v>
       </c>
-      <c r="H244" t="s">
+      <c r="I244" t="s">
         <v>1731</v>
       </c>
-      <c r="I244" t="s">
+      <c r="J244" t="s">
         <v>1732</v>
       </c>
-      <c r="J244" t="s">
+      <c r="K244" t="s">
         <v>1733</v>
-      </c>
-      <c r="K244" t="s">
-        <v>1734</v>
       </c>
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.25">
@@ -15372,25 +15372,25 @@
         <v>7</v>
       </c>
       <c r="D245" t="s">
+        <v>1734</v>
+      </c>
+      <c r="E245" s="1" t="s">
         <v>1735</v>
       </c>
-      <c r="E245" s="1" t="s">
+      <c r="F245" t="s">
         <v>1736</v>
       </c>
-      <c r="F245" t="s">
+      <c r="G245" t="s">
         <v>1737</v>
       </c>
-      <c r="G245" t="s">
+      <c r="H245" t="s">
         <v>1738</v>
       </c>
-      <c r="H245" t="s">
+      <c r="I245" t="s">
         <v>1739</v>
       </c>
-      <c r="I245" t="s">
+      <c r="J245" t="s">
         <v>1740</v>
-      </c>
-      <c r="J245" t="s">
-        <v>1741</v>
       </c>
       <c r="K245" t="s">
         <v>16</v>
@@ -15407,25 +15407,25 @@
         <v>8</v>
       </c>
       <c r="D246" t="s">
+        <v>1741</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>1742</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>1743</v>
       </c>
       <c r="F246" t="s">
         <v>148</v>
       </c>
       <c r="G246" t="s">
+        <v>1743</v>
+      </c>
+      <c r="H246" t="s">
         <v>1744</v>
       </c>
-      <c r="H246" t="s">
+      <c r="I246" t="s">
         <v>1745</v>
       </c>
-      <c r="I246" t="s">
+      <c r="J246" t="s">
         <v>1746</v>
-      </c>
-      <c r="J246" t="s">
-        <v>1747</v>
       </c>
       <c r="K246" t="s">
         <v>16</v>
@@ -15442,28 +15442,28 @@
         <v>9</v>
       </c>
       <c r="D247" t="s">
+        <v>1747</v>
+      </c>
+      <c r="E247" s="1" t="s">
         <v>1748</v>
       </c>
-      <c r="E247" s="1" t="s">
+      <c r="F247" t="s">
         <v>1749</v>
       </c>
-      <c r="F247" t="s">
+      <c r="G247" t="s">
         <v>1750</v>
       </c>
-      <c r="G247" t="s">
+      <c r="H247" t="s">
         <v>1751</v>
       </c>
-      <c r="H247" t="s">
+      <c r="I247" t="s">
         <v>1752</v>
       </c>
-      <c r="I247" t="s">
+      <c r="J247" t="s">
         <v>1753</v>
       </c>
-      <c r="J247" t="s">
+      <c r="K247" t="s">
         <v>1754</v>
-      </c>
-      <c r="K247" t="s">
-        <v>1755</v>
       </c>
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.25">
@@ -15477,25 +15477,25 @@
         <v>10</v>
       </c>
       <c r="D248" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E248" s="1" t="s">
         <v>1756</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>1757</v>
       </c>
       <c r="F248" t="s">
         <v>141</v>
       </c>
       <c r="G248" t="s">
+        <v>1757</v>
+      </c>
+      <c r="H248" t="s">
         <v>1758</v>
       </c>
-      <c r="H248" t="s">
+      <c r="I248" t="s">
         <v>1759</v>
       </c>
-      <c r="I248" t="s">
+      <c r="J248" t="s">
         <v>1760</v>
-      </c>
-      <c r="J248" t="s">
-        <v>1761</v>
       </c>
       <c r="K248" t="s">
         <v>16</v>
@@ -15512,28 +15512,28 @@
         <v>11</v>
       </c>
       <c r="D249" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E249" s="1" t="s">
         <v>1762</v>
       </c>
-      <c r="E249" s="1" t="s">
+      <c r="F249" t="s">
         <v>1763</v>
       </c>
-      <c r="F249" t="s">
+      <c r="G249" t="s">
         <v>1764</v>
       </c>
-      <c r="G249" t="s">
+      <c r="H249" t="s">
         <v>1765</v>
       </c>
-      <c r="H249" t="s">
+      <c r="I249" t="s">
         <v>1766</v>
       </c>
-      <c r="I249" t="s">
+      <c r="J249" t="s">
         <v>1767</v>
       </c>
-      <c r="J249" t="s">
+      <c r="K249" t="s">
         <v>1768</v>
-      </c>
-      <c r="K249" t="s">
-        <v>1769</v>
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.25">
@@ -15547,28 +15547,28 @@
         <v>12</v>
       </c>
       <c r="D250" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>1770</v>
       </c>
-      <c r="E250" s="1" t="s">
+      <c r="F250" t="s">
         <v>1771</v>
       </c>
-      <c r="F250" t="s">
+      <c r="G250" t="s">
         <v>1772</v>
       </c>
-      <c r="G250" t="s">
+      <c r="H250" t="s">
         <v>1773</v>
       </c>
-      <c r="H250" t="s">
+      <c r="I250" t="s">
         <v>1774</v>
       </c>
-      <c r="I250" t="s">
+      <c r="J250" t="s">
         <v>1775</v>
       </c>
-      <c r="J250" t="s">
+      <c r="K250" t="s">
         <v>1776</v>
-      </c>
-      <c r="K250" t="s">
-        <v>1777</v>
       </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.25">
@@ -15582,25 +15582,25 @@
         <v>13</v>
       </c>
       <c r="D251" t="s">
+        <v>1777</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F251" t="s">
         <v>1778</v>
       </c>
-      <c r="E251" s="1" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F251" t="s">
+      <c r="G251" t="s">
         <v>1779</v>
       </c>
-      <c r="G251" t="s">
+      <c r="H251" t="s">
         <v>1780</v>
       </c>
-      <c r="H251" t="s">
+      <c r="I251" t="s">
         <v>1781</v>
       </c>
-      <c r="I251" t="s">
+      <c r="J251" t="s">
         <v>1782</v>
-      </c>
-      <c r="J251" t="s">
-        <v>1783</v>
       </c>
       <c r="K251" t="s">
         <v>16</v>
@@ -15617,25 +15617,25 @@
         <v>1</v>
       </c>
       <c r="D252" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E252" s="1" t="s">
         <v>1784</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>1785</v>
       </c>
       <c r="F252" t="s">
         <v>248</v>
       </c>
       <c r="G252" t="s">
+        <v>1785</v>
+      </c>
+      <c r="H252" t="s">
         <v>1786</v>
       </c>
-      <c r="H252" t="s">
+      <c r="I252" t="s">
         <v>1787</v>
       </c>
-      <c r="I252" t="s">
+      <c r="J252" t="s">
         <v>1788</v>
-      </c>
-      <c r="J252" t="s">
-        <v>1789</v>
       </c>
       <c r="K252" t="s">
         <v>16</v>
@@ -15652,28 +15652,28 @@
         <v>2</v>
       </c>
       <c r="D253" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E253" s="1" t="s">
         <v>1790</v>
       </c>
-      <c r="E253" s="1" t="s">
+      <c r="F253" t="s">
         <v>1791</v>
       </c>
-      <c r="F253" t="s">
+      <c r="G253" t="s">
         <v>1792</v>
       </c>
-      <c r="G253" t="s">
+      <c r="H253" t="s">
         <v>1793</v>
       </c>
-      <c r="H253" t="s">
+      <c r="I253" t="s">
         <v>1794</v>
       </c>
-      <c r="I253" t="s">
+      <c r="J253" t="s">
         <v>1795</v>
       </c>
-      <c r="J253" t="s">
+      <c r="K253" t="s">
         <v>1796</v>
-      </c>
-      <c r="K253" t="s">
-        <v>1797</v>
       </c>
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
@@ -15687,25 +15687,25 @@
         <v>3</v>
       </c>
       <c r="D254" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>1798</v>
       </c>
-      <c r="E254" s="1" t="s">
+      <c r="F254" t="s">
         <v>1799</v>
       </c>
-      <c r="F254" t="s">
+      <c r="G254" t="s">
         <v>1800</v>
       </c>
-      <c r="G254" t="s">
+      <c r="H254" t="s">
         <v>1801</v>
       </c>
-      <c r="H254" t="s">
+      <c r="I254" t="s">
         <v>1802</v>
       </c>
-      <c r="I254" t="s">
+      <c r="J254" t="s">
         <v>1803</v>
-      </c>
-      <c r="J254" t="s">
-        <v>1804</v>
       </c>
       <c r="K254" t="s">
         <v>16</v>
@@ -15722,28 +15722,28 @@
         <v>4</v>
       </c>
       <c r="D255" t="s">
+        <v>1804</v>
+      </c>
+      <c r="E255" s="1" t="s">
         <v>1805</v>
       </c>
-      <c r="E255" s="1" t="s">
+      <c r="F255" t="s">
         <v>1806</v>
       </c>
-      <c r="F255" t="s">
+      <c r="G255" t="s">
         <v>1807</v>
       </c>
-      <c r="G255" t="s">
+      <c r="H255" t="s">
         <v>1808</v>
       </c>
-      <c r="H255" t="s">
+      <c r="I255" t="s">
         <v>1809</v>
       </c>
-      <c r="I255" t="s">
+      <c r="J255" t="s">
         <v>1810</v>
       </c>
-      <c r="J255" t="s">
+      <c r="K255" t="s">
         <v>1811</v>
-      </c>
-      <c r="K255" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.25">
@@ -15757,25 +15757,25 @@
         <v>5</v>
       </c>
       <c r="D256" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E256" s="1" t="s">
         <v>1813</v>
       </c>
-      <c r="E256" s="1" t="s">
+      <c r="F256" t="s">
         <v>1814</v>
       </c>
-      <c r="F256" t="s">
+      <c r="G256" t="s">
         <v>1815</v>
       </c>
-      <c r="G256" t="s">
+      <c r="H256" t="s">
         <v>1816</v>
       </c>
-      <c r="H256" t="s">
+      <c r="I256" t="s">
         <v>1817</v>
       </c>
-      <c r="I256" t="s">
+      <c r="J256" t="s">
         <v>1818</v>
-      </c>
-      <c r="J256" t="s">
-        <v>1819</v>
       </c>
       <c r="K256" t="s">
         <v>16</v>
@@ -15792,28 +15792,28 @@
         <v>6</v>
       </c>
       <c r="D257" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>1820</v>
       </c>
-      <c r="E257" s="1" t="s">
+      <c r="F257" t="s">
         <v>1821</v>
       </c>
-      <c r="F257" t="s">
+      <c r="G257" t="s">
         <v>1822</v>
       </c>
-      <c r="G257" t="s">
+      <c r="H257" t="s">
         <v>1823</v>
       </c>
-      <c r="H257" t="s">
+      <c r="I257" t="s">
         <v>1824</v>
       </c>
-      <c r="I257" t="s">
+      <c r="J257" t="s">
         <v>1825</v>
       </c>
-      <c r="J257" t="s">
+      <c r="K257" t="s">
         <v>1826</v>
-      </c>
-      <c r="K257" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
@@ -15827,25 +15827,25 @@
         <v>7</v>
       </c>
       <c r="D258" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E258" s="1" t="s">
         <v>1828</v>
       </c>
-      <c r="E258" s="1" t="s">
+      <c r="F258" t="s">
         <v>1829</v>
       </c>
-      <c r="F258" t="s">
+      <c r="G258" t="s">
         <v>1830</v>
       </c>
-      <c r="G258" t="s">
+      <c r="H258" t="s">
         <v>1831</v>
       </c>
-      <c r="H258" t="s">
+      <c r="I258" t="s">
         <v>1832</v>
       </c>
-      <c r="I258" t="s">
+      <c r="J258" t="s">
         <v>1833</v>
-      </c>
-      <c r="J258" t="s">
-        <v>1834</v>
       </c>
       <c r="K258" t="s">
         <v>16</v>
@@ -15862,25 +15862,25 @@
         <v>8</v>
       </c>
       <c r="D259" t="s">
+        <v>1834</v>
+      </c>
+      <c r="E259" s="1" t="s">
         <v>1835</v>
       </c>
-      <c r="E259" s="1" t="s">
+      <c r="F259" t="s">
         <v>1836</v>
       </c>
-      <c r="F259" t="s">
+      <c r="G259" t="s">
         <v>1837</v>
       </c>
-      <c r="G259" t="s">
+      <c r="H259" t="s">
         <v>1838</v>
       </c>
-      <c r="H259" t="s">
+      <c r="I259" t="s">
         <v>1839</v>
       </c>
-      <c r="I259" t="s">
+      <c r="J259" t="s">
         <v>1840</v>
-      </c>
-      <c r="J259" t="s">
-        <v>1841</v>
       </c>
       <c r="K259" t="s">
         <v>16</v>
@@ -15897,25 +15897,25 @@
         <v>9</v>
       </c>
       <c r="D260" t="s">
+        <v>1841</v>
+      </c>
+      <c r="E260" s="1" t="s">
         <v>1842</v>
       </c>
-      <c r="E260" s="1" t="s">
+      <c r="F260" t="s">
         <v>1843</v>
       </c>
-      <c r="F260" t="s">
+      <c r="G260" t="s">
         <v>1844</v>
       </c>
-      <c r="G260" t="s">
+      <c r="H260" t="s">
         <v>1845</v>
       </c>
-      <c r="H260" t="s">
+      <c r="I260" t="s">
         <v>1846</v>
       </c>
-      <c r="I260" t="s">
+      <c r="J260" t="s">
         <v>1847</v>
-      </c>
-      <c r="J260" t="s">
-        <v>1848</v>
       </c>
       <c r="K260" t="s">
         <v>16</v>
@@ -15932,28 +15932,28 @@
         <v>1</v>
       </c>
       <c r="D261" t="s">
+        <v>1848</v>
+      </c>
+      <c r="E261" s="1" t="s">
         <v>1849</v>
       </c>
-      <c r="E261" s="1" t="s">
+      <c r="F261" t="s">
         <v>1850</v>
       </c>
-      <c r="F261" t="s">
+      <c r="G261" t="s">
         <v>1851</v>
       </c>
-      <c r="G261" t="s">
+      <c r="H261" t="s">
         <v>1852</v>
       </c>
-      <c r="H261" t="s">
+      <c r="I261" t="s">
         <v>1853</v>
       </c>
-      <c r="I261" t="s">
+      <c r="J261" t="s">
         <v>1854</v>
       </c>
-      <c r="J261" t="s">
+      <c r="K261" t="s">
         <v>1855</v>
-      </c>
-      <c r="K261" t="s">
-        <v>1856</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
@@ -15967,22 +15967,22 @@
         <v>2</v>
       </c>
       <c r="D262" t="s">
+        <v>1856</v>
+      </c>
+      <c r="E262" s="1" t="s">
         <v>1857</v>
       </c>
-      <c r="E262" s="1" t="s">
+      <c r="F262" t="s">
+        <v>2147</v>
+      </c>
+      <c r="G262" t="s">
         <v>1858</v>
       </c>
-      <c r="F262" t="s">
-        <v>2148</v>
-      </c>
-      <c r="G262" t="s">
+      <c r="H262" t="s">
         <v>1859</v>
       </c>
-      <c r="H262" t="s">
+      <c r="I262" t="s">
         <v>1860</v>
-      </c>
-      <c r="I262" t="s">
-        <v>1861</v>
       </c>
       <c r="J262" t="s">
         <v>1043</v>
@@ -16002,28 +16002,28 @@
         <v>3</v>
       </c>
       <c r="D263" t="s">
+        <v>1861</v>
+      </c>
+      <c r="E263" s="1" t="s">
         <v>1862</v>
       </c>
-      <c r="E263" s="1" t="s">
+      <c r="F263" t="s">
         <v>1863</v>
       </c>
-      <c r="F263" t="s">
+      <c r="G263" t="s">
         <v>1864</v>
       </c>
-      <c r="G263" t="s">
+      <c r="H263" t="s">
         <v>1865</v>
       </c>
-      <c r="H263" t="s">
+      <c r="I263" t="s">
         <v>1866</v>
       </c>
-      <c r="I263" t="s">
+      <c r="J263" t="s">
         <v>1867</v>
       </c>
-      <c r="J263" t="s">
+      <c r="K263" t="s">
         <v>1868</v>
-      </c>
-      <c r="K263" t="s">
-        <v>1869</v>
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
@@ -16037,25 +16037,25 @@
         <v>4</v>
       </c>
       <c r="D264" t="s">
+        <v>1869</v>
+      </c>
+      <c r="E264" s="1" t="s">
         <v>1870</v>
       </c>
-      <c r="E264" s="1" t="s">
+      <c r="F264" t="s">
         <v>1871</v>
       </c>
-      <c r="F264" t="s">
+      <c r="G264" t="s">
         <v>1872</v>
       </c>
-      <c r="G264" t="s">
+      <c r="H264" t="s">
         <v>1873</v>
       </c>
-      <c r="H264" t="s">
+      <c r="I264" t="s">
         <v>1874</v>
       </c>
-      <c r="I264" t="s">
+      <c r="J264" t="s">
         <v>1875</v>
-      </c>
-      <c r="J264" t="s">
-        <v>1876</v>
       </c>
       <c r="K264" t="s">
         <v>16</v>
@@ -16072,25 +16072,25 @@
         <v>5</v>
       </c>
       <c r="D265" t="s">
+        <v>1876</v>
+      </c>
+      <c r="E265" s="1" t="s">
         <v>1877</v>
       </c>
-      <c r="E265" s="1" t="s">
+      <c r="F265" t="s">
         <v>1878</v>
       </c>
-      <c r="F265" t="s">
+      <c r="G265" t="s">
         <v>1879</v>
       </c>
-      <c r="G265" t="s">
+      <c r="H265" t="s">
         <v>1880</v>
       </c>
-      <c r="H265" t="s">
+      <c r="I265" t="s">
         <v>1881</v>
       </c>
-      <c r="I265" t="s">
+      <c r="J265" t="s">
         <v>1882</v>
-      </c>
-      <c r="J265" t="s">
-        <v>1883</v>
       </c>
       <c r="K265" t="s">
         <v>16</v>
@@ -16107,25 +16107,25 @@
         <v>6</v>
       </c>
       <c r="D266" t="s">
+        <v>1883</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="F266" t="s">
         <v>1884</v>
       </c>
-      <c r="E266" s="1" t="s">
-        <v>1878</v>
-      </c>
-      <c r="F266" t="s">
+      <c r="G266" t="s">
         <v>1885</v>
       </c>
-      <c r="G266" t="s">
+      <c r="H266" t="s">
         <v>1886</v>
       </c>
-      <c r="H266" t="s">
+      <c r="I266" t="s">
         <v>1887</v>
       </c>
-      <c r="I266" t="s">
+      <c r="J266" t="s">
         <v>1888</v>
-      </c>
-      <c r="J266" t="s">
-        <v>1889</v>
       </c>
       <c r="K266" t="s">
         <v>16</v>
@@ -16142,25 +16142,25 @@
         <v>7</v>
       </c>
       <c r="D267" t="s">
+        <v>1889</v>
+      </c>
+      <c r="E267" s="1" t="s">
         <v>1890</v>
       </c>
-      <c r="E267" s="1" t="s">
+      <c r="F267" t="s">
         <v>1891</v>
       </c>
-      <c r="F267" t="s">
+      <c r="G267" t="s">
         <v>1892</v>
       </c>
-      <c r="G267" t="s">
+      <c r="H267" t="s">
         <v>1893</v>
       </c>
-      <c r="H267" t="s">
+      <c r="I267" t="s">
         <v>1894</v>
       </c>
-      <c r="I267" t="s">
+      <c r="J267" t="s">
         <v>1895</v>
-      </c>
-      <c r="J267" t="s">
-        <v>1896</v>
       </c>
       <c r="K267" t="s">
         <v>16</v>
@@ -16177,28 +16177,28 @@
         <v>8</v>
       </c>
       <c r="D268" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E268" s="1" t="s">
         <v>1897</v>
       </c>
-      <c r="E268" s="1" t="s">
+      <c r="F268" t="s">
         <v>1898</v>
       </c>
-      <c r="F268" t="s">
+      <c r="G268" t="s">
         <v>1899</v>
       </c>
-      <c r="G268" t="s">
+      <c r="H268" t="s">
         <v>1900</v>
       </c>
-      <c r="H268" t="s">
+      <c r="I268" t="s">
         <v>1901</v>
       </c>
-      <c r="I268" t="s">
+      <c r="J268" t="s">
         <v>1902</v>
       </c>
-      <c r="J268" t="s">
+      <c r="K268" t="s">
         <v>1903</v>
-      </c>
-      <c r="K268" t="s">
-        <v>1904</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
@@ -16212,25 +16212,25 @@
         <v>9</v>
       </c>
       <c r="D269" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E269" s="1" t="s">
         <v>1905</v>
       </c>
-      <c r="E269" s="1" t="s">
+      <c r="F269" t="s">
         <v>1906</v>
       </c>
-      <c r="F269" t="s">
+      <c r="G269" t="s">
         <v>1907</v>
       </c>
-      <c r="G269" t="s">
+      <c r="H269" t="s">
         <v>1908</v>
       </c>
-      <c r="H269" t="s">
+      <c r="I269" t="s">
         <v>1909</v>
       </c>
-      <c r="I269" t="s">
+      <c r="J269" t="s">
         <v>1910</v>
-      </c>
-      <c r="J269" t="s">
-        <v>1911</v>
       </c>
       <c r="K269" t="s">
         <v>16</v>
@@ -16247,28 +16247,28 @@
         <v>10</v>
       </c>
       <c r="D270" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E270" s="1" t="s">
         <v>1912</v>
       </c>
-      <c r="E270" s="1" t="s">
+      <c r="F270" t="s">
         <v>1913</v>
       </c>
-      <c r="F270" t="s">
+      <c r="G270" t="s">
         <v>1914</v>
       </c>
-      <c r="G270" t="s">
+      <c r="H270" t="s">
         <v>1915</v>
       </c>
-      <c r="H270" t="s">
+      <c r="I270" t="s">
         <v>1916</v>
       </c>
-      <c r="I270" t="s">
+      <c r="J270" t="s">
         <v>1917</v>
       </c>
-      <c r="J270" t="s">
+      <c r="K270" t="s">
         <v>1918</v>
-      </c>
-      <c r="K270" t="s">
-        <v>1919</v>
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
@@ -16282,25 +16282,25 @@
         <v>11</v>
       </c>
       <c r="D271" t="s">
+        <v>1919</v>
+      </c>
+      <c r="E271" s="1" t="s">
         <v>1920</v>
       </c>
-      <c r="E271" s="1" t="s">
+      <c r="F271" t="s">
         <v>1921</v>
       </c>
-      <c r="F271" t="s">
+      <c r="G271" t="s">
         <v>1922</v>
       </c>
-      <c r="G271" t="s">
+      <c r="H271" t="s">
         <v>1923</v>
       </c>
-      <c r="H271" t="s">
+      <c r="I271" t="s">
         <v>1924</v>
       </c>
-      <c r="I271" t="s">
+      <c r="J271" t="s">
         <v>1925</v>
-      </c>
-      <c r="J271" t="s">
-        <v>1926</v>
       </c>
       <c r="K271" t="s">
         <v>16</v>
@@ -16317,25 +16317,25 @@
         <v>12</v>
       </c>
       <c r="D272" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E272" s="1" t="s">
         <v>1927</v>
       </c>
-      <c r="E272" s="1" t="s">
+      <c r="F272" t="s">
         <v>1928</v>
       </c>
-      <c r="F272" t="s">
+      <c r="G272" t="s">
         <v>1929</v>
       </c>
-      <c r="G272" t="s">
+      <c r="H272" t="s">
         <v>1930</v>
       </c>
-      <c r="H272" t="s">
+      <c r="I272" t="s">
         <v>1931</v>
       </c>
-      <c r="I272" t="s">
+      <c r="J272" t="s">
         <v>1932</v>
-      </c>
-      <c r="J272" t="s">
-        <v>1933</v>
       </c>
       <c r="K272" t="s">
         <v>16</v>
@@ -16352,25 +16352,25 @@
         <v>13</v>
       </c>
       <c r="D273" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E273" s="1" t="s">
         <v>1934</v>
       </c>
-      <c r="E273" s="1" t="s">
+      <c r="F273" t="s">
         <v>1935</v>
       </c>
-      <c r="F273" t="s">
+      <c r="G273" t="s">
         <v>1936</v>
       </c>
-      <c r="G273" t="s">
+      <c r="H273" t="s">
         <v>1937</v>
       </c>
-      <c r="H273" t="s">
+      <c r="I273" t="s">
         <v>1938</v>
       </c>
-      <c r="I273" t="s">
+      <c r="J273" t="s">
         <v>1939</v>
-      </c>
-      <c r="J273" t="s">
-        <v>1940</v>
       </c>
       <c r="K273" t="s">
         <v>16</v>
@@ -16387,28 +16387,28 @@
         <v>1</v>
       </c>
       <c r="D274" t="s">
+        <v>1940</v>
+      </c>
+      <c r="E274" s="1" t="s">
         <v>1941</v>
       </c>
-      <c r="E274" s="1" t="s">
+      <c r="F274" t="s">
         <v>1942</v>
       </c>
-      <c r="F274" t="s">
+      <c r="G274" t="s">
         <v>1943</v>
       </c>
-      <c r="G274" t="s">
+      <c r="H274" t="s">
         <v>1944</v>
       </c>
-      <c r="H274" t="s">
+      <c r="I274" t="s">
         <v>1945</v>
       </c>
-      <c r="I274" t="s">
+      <c r="J274" t="s">
         <v>1946</v>
       </c>
-      <c r="J274" t="s">
+      <c r="K274" t="s">
         <v>1947</v>
-      </c>
-      <c r="K274" t="s">
-        <v>1948</v>
       </c>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.25">
@@ -16422,25 +16422,25 @@
         <v>2</v>
       </c>
       <c r="D275" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E275" s="1" t="s">
         <v>1949</v>
       </c>
-      <c r="E275" s="1" t="s">
+      <c r="F275" t="s">
         <v>1950</v>
       </c>
-      <c r="F275" t="s">
+      <c r="G275" t="s">
         <v>1951</v>
       </c>
-      <c r="G275" t="s">
+      <c r="H275" t="s">
         <v>1952</v>
       </c>
-      <c r="H275" t="s">
+      <c r="I275" t="s">
         <v>1953</v>
       </c>
-      <c r="I275" t="s">
+      <c r="J275" t="s">
         <v>1954</v>
-      </c>
-      <c r="J275" t="s">
-        <v>1955</v>
       </c>
       <c r="K275" t="s">
         <v>16</v>
@@ -16457,28 +16457,28 @@
         <v>3</v>
       </c>
       <c r="D276" t="s">
+        <v>1955</v>
+      </c>
+      <c r="E276" s="1" t="s">
         <v>1956</v>
       </c>
-      <c r="E276" s="1" t="s">
+      <c r="F276" t="s">
         <v>1957</v>
       </c>
-      <c r="F276" t="s">
+      <c r="G276" t="s">
         <v>1958</v>
       </c>
-      <c r="G276" t="s">
+      <c r="H276" t="s">
         <v>1959</v>
       </c>
-      <c r="H276" t="s">
+      <c r="I276" t="s">
         <v>1960</v>
       </c>
-      <c r="I276" t="s">
+      <c r="J276" t="s">
         <v>1961</v>
       </c>
-      <c r="J276" t="s">
+      <c r="K276" t="s">
         <v>1962</v>
-      </c>
-      <c r="K276" t="s">
-        <v>1963</v>
       </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
@@ -16492,28 +16492,28 @@
         <v>4</v>
       </c>
       <c r="D277" t="s">
+        <v>1963</v>
+      </c>
+      <c r="E277" s="1" t="s">
         <v>1964</v>
       </c>
-      <c r="E277" s="1" t="s">
+      <c r="F277" t="s">
         <v>1965</v>
       </c>
-      <c r="F277" t="s">
+      <c r="G277" t="s">
         <v>1966</v>
       </c>
-      <c r="G277" t="s">
+      <c r="H277" t="s">
         <v>1967</v>
       </c>
-      <c r="H277" t="s">
+      <c r="I277" t="s">
         <v>1968</v>
       </c>
-      <c r="I277" t="s">
+      <c r="J277" t="s">
         <v>1969</v>
       </c>
-      <c r="J277" t="s">
+      <c r="K277" t="s">
         <v>1970</v>
-      </c>
-      <c r="K277" t="s">
-        <v>1971</v>
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
@@ -16527,25 +16527,25 @@
         <v>5</v>
       </c>
       <c r="D278" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E278" s="1" t="s">
         <v>1972</v>
       </c>
-      <c r="E278" s="1" t="s">
+      <c r="F278" t="s">
         <v>1973</v>
       </c>
-      <c r="F278" t="s">
+      <c r="G278" t="s">
         <v>1974</v>
       </c>
-      <c r="G278" t="s">
+      <c r="H278" t="s">
         <v>1975</v>
       </c>
-      <c r="H278" t="s">
+      <c r="I278" t="s">
         <v>1976</v>
       </c>
-      <c r="I278" t="s">
+      <c r="J278" t="s">
         <v>1977</v>
-      </c>
-      <c r="J278" t="s">
-        <v>1978</v>
       </c>
       <c r="K278" t="s">
         <v>16</v>
@@ -16562,28 +16562,28 @@
         <v>6</v>
       </c>
       <c r="D279" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E279" s="1" t="s">
         <v>1979</v>
       </c>
-      <c r="E279" s="1" t="s">
+      <c r="F279" t="s">
         <v>1980</v>
       </c>
-      <c r="F279" t="s">
+      <c r="G279" t="s">
         <v>1981</v>
       </c>
-      <c r="G279" t="s">
+      <c r="H279" t="s">
         <v>1982</v>
       </c>
-      <c r="H279" t="s">
+      <c r="I279" t="s">
         <v>1983</v>
       </c>
-      <c r="I279" t="s">
+      <c r="J279" t="s">
         <v>1984</v>
       </c>
-      <c r="J279" t="s">
+      <c r="K279" t="s">
         <v>1985</v>
-      </c>
-      <c r="K279" t="s">
-        <v>1986</v>
       </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.25">
@@ -16597,25 +16597,25 @@
         <v>7</v>
       </c>
       <c r="D280" t="s">
+        <v>1986</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F280" t="s">
         <v>1987</v>
       </c>
-      <c r="E280" s="1" t="s">
-        <v>1980</v>
-      </c>
-      <c r="F280" t="s">
+      <c r="G280" t="s">
         <v>1988</v>
       </c>
-      <c r="G280" t="s">
+      <c r="H280" t="s">
         <v>1989</v>
       </c>
-      <c r="H280" t="s">
+      <c r="I280" t="s">
         <v>1990</v>
       </c>
-      <c r="I280" t="s">
+      <c r="J280" t="s">
         <v>1991</v>
-      </c>
-      <c r="J280" t="s">
-        <v>1992</v>
       </c>
       <c r="K280" t="s">
         <v>16</v>
@@ -16632,28 +16632,28 @@
         <v>8</v>
       </c>
       <c r="D281" t="s">
+        <v>1992</v>
+      </c>
+      <c r="E281" s="1" t="s">
         <v>1993</v>
       </c>
-      <c r="E281" s="1" t="s">
+      <c r="F281" t="s">
         <v>1994</v>
       </c>
-      <c r="F281" t="s">
+      <c r="G281" t="s">
         <v>1995</v>
       </c>
-      <c r="G281" t="s">
+      <c r="H281" t="s">
         <v>1996</v>
       </c>
-      <c r="H281" t="s">
+      <c r="I281" t="s">
         <v>1997</v>
       </c>
-      <c r="I281" t="s">
+      <c r="J281" t="s">
         <v>1998</v>
       </c>
-      <c r="J281" t="s">
+      <c r="K281" t="s">
         <v>1999</v>
-      </c>
-      <c r="K281" t="s">
-        <v>2000</v>
       </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
@@ -16667,25 +16667,25 @@
         <v>9</v>
       </c>
       <c r="D282" t="s">
+        <v>2000</v>
+      </c>
+      <c r="E282" s="1" t="s">
         <v>2001</v>
       </c>
-      <c r="E282" s="1" t="s">
+      <c r="F282" t="s">
         <v>2002</v>
       </c>
-      <c r="F282" t="s">
+      <c r="G282" t="s">
         <v>2003</v>
       </c>
-      <c r="G282" t="s">
+      <c r="H282" t="s">
         <v>2004</v>
       </c>
-      <c r="H282" t="s">
+      <c r="I282" t="s">
         <v>2005</v>
       </c>
-      <c r="I282" t="s">
+      <c r="J282" t="s">
         <v>2006</v>
-      </c>
-      <c r="J282" t="s">
-        <v>2007</v>
       </c>
       <c r="K282" t="s">
         <v>16</v>
@@ -16702,28 +16702,28 @@
         <v>10</v>
       </c>
       <c r="D283" t="s">
+        <v>2007</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F283" t="s">
         <v>2008</v>
       </c>
-      <c r="E283" s="1" t="s">
-        <v>2002</v>
-      </c>
-      <c r="F283" t="s">
+      <c r="G283" t="s">
         <v>2009</v>
       </c>
-      <c r="G283" t="s">
+      <c r="H283" t="s">
         <v>2010</v>
       </c>
-      <c r="H283" t="s">
+      <c r="I283" t="s">
         <v>2011</v>
       </c>
-      <c r="I283" t="s">
+      <c r="J283" t="s">
         <v>2012</v>
       </c>
-      <c r="J283" t="s">
+      <c r="K283" t="s">
         <v>2013</v>
-      </c>
-      <c r="K283" t="s">
-        <v>2014</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
@@ -16737,25 +16737,25 @@
         <v>11</v>
       </c>
       <c r="D284" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E284" s="1" t="s">
         <v>2015</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="F284" t="s">
         <v>2016</v>
       </c>
-      <c r="F284" t="s">
+      <c r="G284" t="s">
         <v>2017</v>
       </c>
-      <c r="G284" t="s">
+      <c r="H284" t="s">
         <v>2018</v>
       </c>
-      <c r="H284" t="s">
+      <c r="I284" t="s">
         <v>2019</v>
       </c>
-      <c r="I284" t="s">
+      <c r="J284" t="s">
         <v>2020</v>
-      </c>
-      <c r="J284" t="s">
-        <v>2021</v>
       </c>
       <c r="K284" t="s">
         <v>16</v>
@@ -16772,25 +16772,25 @@
         <v>12</v>
       </c>
       <c r="D285" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>2015</v>
+      </c>
+      <c r="F285" t="s">
         <v>2022</v>
       </c>
-      <c r="E285" s="1" t="s">
-        <v>2016</v>
-      </c>
-      <c r="F285" t="s">
+      <c r="G285" t="s">
         <v>2023</v>
       </c>
-      <c r="G285" t="s">
+      <c r="H285" t="s">
         <v>2024</v>
       </c>
-      <c r="H285" t="s">
+      <c r="I285" t="s">
         <v>2025</v>
       </c>
-      <c r="I285" t="s">
+      <c r="J285" t="s">
         <v>2026</v>
-      </c>
-      <c r="J285" t="s">
-        <v>2027</v>
       </c>
       <c r="K285" t="s">
         <v>16</v>
@@ -16807,28 +16807,28 @@
         <v>1</v>
       </c>
       <c r="D286" t="s">
+        <v>2027</v>
+      </c>
+      <c r="E286" s="1" t="s">
         <v>2028</v>
       </c>
-      <c r="E286" s="1" t="s">
+      <c r="F286" t="s">
         <v>2029</v>
       </c>
-      <c r="F286" t="s">
+      <c r="G286" t="s">
         <v>2030</v>
       </c>
-      <c r="G286" t="s">
+      <c r="H286" t="s">
         <v>2031</v>
       </c>
-      <c r="H286" t="s">
+      <c r="I286" t="s">
         <v>2032</v>
       </c>
-      <c r="I286" t="s">
+      <c r="J286" t="s">
         <v>2033</v>
       </c>
-      <c r="J286" t="s">
+      <c r="K286" t="s">
         <v>2034</v>
-      </c>
-      <c r="K286" t="s">
-        <v>2035</v>
       </c>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.25">
@@ -16842,28 +16842,28 @@
         <v>2</v>
       </c>
       <c r="D287" t="s">
+        <v>2035</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="F287" t="s">
         <v>2036</v>
       </c>
-      <c r="E287" s="1" t="s">
-        <v>2029</v>
-      </c>
-      <c r="F287" t="s">
+      <c r="G287" t="s">
         <v>2037</v>
       </c>
-      <c r="G287" t="s">
+      <c r="H287" t="s">
         <v>2038</v>
       </c>
-      <c r="H287" t="s">
+      <c r="I287" t="s">
         <v>2039</v>
       </c>
-      <c r="I287" t="s">
+      <c r="J287" t="s">
         <v>2040</v>
       </c>
-      <c r="J287" t="s">
+      <c r="K287" t="s">
         <v>2041</v>
-      </c>
-      <c r="K287" t="s">
-        <v>2042</v>
       </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.25">
@@ -16877,28 +16877,28 @@
         <v>3</v>
       </c>
       <c r="D288" t="s">
+        <v>2042</v>
+      </c>
+      <c r="E288" s="1" t="s">
         <v>2043</v>
       </c>
-      <c r="E288" s="1" t="s">
+      <c r="F288" t="s">
         <v>2044</v>
       </c>
-      <c r="F288" t="s">
+      <c r="G288" t="s">
         <v>2045</v>
       </c>
-      <c r="G288" t="s">
+      <c r="H288" t="s">
         <v>2046</v>
       </c>
-      <c r="H288" t="s">
+      <c r="I288" t="s">
         <v>2047</v>
       </c>
-      <c r="I288" t="s">
+      <c r="J288" t="s">
         <v>2048</v>
       </c>
-      <c r="J288" t="s">
+      <c r="K288" t="s">
         <v>2049</v>
-      </c>
-      <c r="K288" t="s">
-        <v>2050</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.25">
@@ -16912,25 +16912,25 @@
         <v>4</v>
       </c>
       <c r="D289" t="s">
+        <v>2050</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>2043</v>
+      </c>
+      <c r="F289" t="s">
         <v>2051</v>
       </c>
-      <c r="E289" s="1" t="s">
-        <v>2044</v>
-      </c>
-      <c r="F289" t="s">
+      <c r="G289" t="s">
         <v>2052</v>
       </c>
-      <c r="G289" t="s">
+      <c r="H289" t="s">
         <v>2053</v>
       </c>
-      <c r="H289" t="s">
+      <c r="I289" t="s">
         <v>2054</v>
       </c>
-      <c r="I289" t="s">
+      <c r="J289" t="s">
         <v>2055</v>
-      </c>
-      <c r="J289" t="s">
-        <v>2056</v>
       </c>
       <c r="K289" t="s">
         <v>16</v>
@@ -16947,28 +16947,28 @@
         <v>5</v>
       </c>
       <c r="D290" t="s">
+        <v>2056</v>
+      </c>
+      <c r="E290" s="1" t="s">
         <v>2057</v>
       </c>
-      <c r="E290" s="1" t="s">
+      <c r="F290" t="s">
         <v>2058</v>
       </c>
-      <c r="F290" t="s">
+      <c r="G290" t="s">
         <v>2059</v>
       </c>
-      <c r="G290" t="s">
+      <c r="H290" t="s">
         <v>2060</v>
       </c>
-      <c r="H290" t="s">
+      <c r="I290" t="s">
         <v>2061</v>
       </c>
-      <c r="I290" t="s">
+      <c r="J290" t="s">
         <v>2062</v>
       </c>
-      <c r="J290" t="s">
+      <c r="K290" t="s">
         <v>2063</v>
-      </c>
-      <c r="K290" t="s">
-        <v>2064</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.25">
@@ -16982,25 +16982,25 @@
         <v>6</v>
       </c>
       <c r="D291" t="s">
+        <v>2064</v>
+      </c>
+      <c r="E291" s="1" t="s">
         <v>2065</v>
       </c>
-      <c r="E291" s="1" t="s">
+      <c r="F291" t="s">
         <v>2066</v>
       </c>
-      <c r="F291" t="s">
+      <c r="G291" t="s">
         <v>2067</v>
       </c>
-      <c r="G291" t="s">
+      <c r="H291" t="s">
         <v>2068</v>
       </c>
-      <c r="H291" t="s">
+      <c r="I291" t="s">
         <v>2069</v>
       </c>
-      <c r="I291" t="s">
+      <c r="J291" t="s">
         <v>2070</v>
-      </c>
-      <c r="J291" t="s">
-        <v>2071</v>
       </c>
       <c r="K291" t="s">
         <v>16</v>
@@ -17017,25 +17017,25 @@
         <v>7</v>
       </c>
       <c r="D292" t="s">
+        <v>2071</v>
+      </c>
+      <c r="E292" s="1" t="s">
         <v>2072</v>
       </c>
-      <c r="E292" s="1" t="s">
+      <c r="F292" t="s">
         <v>2073</v>
       </c>
-      <c r="F292" t="s">
+      <c r="G292" t="s">
         <v>2074</v>
       </c>
-      <c r="G292" t="s">
+      <c r="H292" t="s">
         <v>2075</v>
       </c>
-      <c r="H292" t="s">
+      <c r="I292" t="s">
         <v>2076</v>
       </c>
-      <c r="I292" t="s">
+      <c r="J292" t="s">
         <v>2077</v>
-      </c>
-      <c r="J292" t="s">
-        <v>2078</v>
       </c>
       <c r="K292" t="s">
         <v>16</v>
@@ -17052,28 +17052,28 @@
         <v>8</v>
       </c>
       <c r="D293" t="s">
+        <v>2078</v>
+      </c>
+      <c r="E293" s="1" t="s">
         <v>2079</v>
       </c>
-      <c r="E293" s="1" t="s">
+      <c r="F293" t="s">
         <v>2080</v>
       </c>
-      <c r="F293" t="s">
+      <c r="G293" t="s">
         <v>2081</v>
       </c>
-      <c r="G293" t="s">
+      <c r="H293" t="s">
         <v>2082</v>
       </c>
-      <c r="H293" t="s">
+      <c r="I293" t="s">
         <v>2083</v>
       </c>
-      <c r="I293" t="s">
+      <c r="J293" t="s">
         <v>2084</v>
       </c>
-      <c r="J293" t="s">
+      <c r="K293" t="s">
         <v>2085</v>
-      </c>
-      <c r="K293" t="s">
-        <v>2086</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">
@@ -17087,25 +17087,25 @@
         <v>9</v>
       </c>
       <c r="D294" t="s">
+        <v>2086</v>
+      </c>
+      <c r="E294" s="1" t="s">
         <v>2087</v>
       </c>
-      <c r="E294" s="1" t="s">
+      <c r="F294" t="s">
         <v>2088</v>
       </c>
-      <c r="F294" t="s">
+      <c r="G294" t="s">
         <v>2089</v>
       </c>
-      <c r="G294" t="s">
+      <c r="H294" t="s">
         <v>2090</v>
       </c>
-      <c r="H294" t="s">
+      <c r="I294" t="s">
         <v>2091</v>
       </c>
-      <c r="I294" t="s">
+      <c r="J294" t="s">
         <v>2092</v>
-      </c>
-      <c r="J294" t="s">
-        <v>2093</v>
       </c>
       <c r="K294" t="s">
         <v>16</v>
@@ -17122,28 +17122,28 @@
         <v>10</v>
       </c>
       <c r="D295" t="s">
+        <v>2093</v>
+      </c>
+      <c r="E295" s="1" t="s">
         <v>2094</v>
       </c>
-      <c r="E295" s="1" t="s">
+      <c r="F295" t="s">
         <v>2095</v>
       </c>
-      <c r="F295" t="s">
+      <c r="G295" t="s">
         <v>2096</v>
       </c>
-      <c r="G295" t="s">
+      <c r="H295" t="s">
         <v>2097</v>
       </c>
-      <c r="H295" t="s">
+      <c r="I295" t="s">
         <v>2098</v>
       </c>
-      <c r="I295" t="s">
+      <c r="J295" t="s">
         <v>2099</v>
       </c>
-      <c r="J295" t="s">
+      <c r="K295" t="s">
         <v>2100</v>
-      </c>
-      <c r="K295" t="s">
-        <v>2101</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.25">
@@ -17157,25 +17157,25 @@
         <v>11</v>
       </c>
       <c r="D296" t="s">
+        <v>2101</v>
+      </c>
+      <c r="E296" s="1" t="s">
         <v>2102</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>2103</v>
       </c>
       <c r="F296" t="s">
         <v>1082</v>
       </c>
       <c r="G296" t="s">
+        <v>2103</v>
+      </c>
+      <c r="H296" t="s">
         <v>2104</v>
       </c>
-      <c r="H296" t="s">
+      <c r="I296" t="s">
         <v>2105</v>
       </c>
-      <c r="I296" t="s">
+      <c r="J296" t="s">
         <v>2106</v>
-      </c>
-      <c r="J296" t="s">
-        <v>2107</v>
       </c>
       <c r="K296" t="s">
         <v>16</v>
@@ -17192,28 +17192,28 @@
         <v>12</v>
       </c>
       <c r="D297" t="s">
+        <v>2107</v>
+      </c>
+      <c r="E297" s="1" t="s">
         <v>2108</v>
       </c>
-      <c r="E297" s="1" t="s">
+      <c r="F297" t="s">
+        <v>1401</v>
+      </c>
+      <c r="G297" t="s">
         <v>2109</v>
       </c>
-      <c r="F297" t="s">
-        <v>1402</v>
-      </c>
-      <c r="G297" t="s">
+      <c r="H297" t="s">
         <v>2110</v>
       </c>
-      <c r="H297" t="s">
+      <c r="I297" t="s">
         <v>2111</v>
       </c>
-      <c r="I297" t="s">
+      <c r="J297" t="s">
         <v>2112</v>
       </c>
-      <c r="J297" t="s">
+      <c r="K297" t="s">
         <v>2113</v>
-      </c>
-      <c r="K297" t="s">
-        <v>2114</v>
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.25">
@@ -17227,28 +17227,28 @@
         <v>13</v>
       </c>
       <c r="D298" t="s">
+        <v>2114</v>
+      </c>
+      <c r="E298" s="1" t="s">
         <v>2115</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>2116</v>
       </c>
       <c r="F298" t="s">
         <v>669</v>
       </c>
       <c r="G298" t="s">
+        <v>2116</v>
+      </c>
+      <c r="H298" t="s">
+        <v>1728</v>
+      </c>
+      <c r="I298" t="s">
         <v>2117</v>
       </c>
-      <c r="H298" t="s">
-        <v>1729</v>
-      </c>
-      <c r="I298" t="s">
+      <c r="J298" t="s">
         <v>2118</v>
       </c>
-      <c r="J298" t="s">
+      <c r="K298" t="s">
         <v>2119</v>
-      </c>
-      <c r="K298" t="s">
-        <v>2120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>